<commit_message>
Update NM materiais do SMS SI.xlsx
</commit_message>
<xml_diff>
--- a/NM materiais do SMS SI.xlsx
+++ b/NM materiais do SMS SI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\Controle Materiais Estoque\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petrobrasbr-my.sharepoint.com/personal/afonsoverardi_prestserv_petrobras_com_br/Documents/Documentos/GitHub/dashboard-estoque/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBAD423-F720-4E46-89A9-50B15EC4CCB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{8FBAD423-F720-4E46-89A9-50B15EC4CCB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DDA7FB4-506A-4E15-9242-ADCD6A9E59D6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="114">
   <si>
     <t>Derivante esfér.fech.ráp. p/mang.incên.</t>
   </si>
@@ -357,9 +357,6 @@
   </si>
   <si>
     <t>11.158.686</t>
-  </si>
-  <si>
-    <t>11.245.954</t>
   </si>
   <si>
     <t>11.283.594</t>
@@ -750,6 +747,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
@@ -1037,10 +1038,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,13 +1056,13 @@
         <v>51</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C1" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="26" t="s">
         <v>107</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1072,10 +1073,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1086,10 +1087,10 @@
         <v>0</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1100,10 +1101,10 @@
         <v>34</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1114,10 +1115,10 @@
         <v>26</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1128,10 +1129,10 @@
         <v>32</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1142,10 +1143,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1156,10 +1157,10 @@
         <v>19</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1170,10 +1171,10 @@
         <v>35</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1184,10 +1185,10 @@
         <v>15</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1198,10 +1199,10 @@
         <v>43</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1212,10 +1213,10 @@
         <v>36</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1226,10 +1227,10 @@
         <v>23</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1240,10 +1241,10 @@
         <v>33</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1254,10 +1255,10 @@
         <v>8</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1268,10 +1269,10 @@
         <v>25</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1282,10 +1283,10 @@
         <v>14</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1296,10 +1297,10 @@
         <v>16</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1310,10 +1311,10 @@
         <v>6</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1324,10 +1325,10 @@
         <v>27</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1338,10 +1339,10 @@
         <v>7</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1352,10 +1353,10 @@
         <v>48</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1366,10 +1367,10 @@
         <v>50</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1380,10 +1381,10 @@
         <v>28</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1394,10 +1395,10 @@
         <v>18</v>
       </c>
       <c r="C25" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1408,10 +1409,10 @@
         <v>9</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1422,10 +1423,10 @@
         <v>24</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1436,10 +1437,10 @@
         <v>38</v>
       </c>
       <c r="C28" s="33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1450,10 +1451,10 @@
         <v>10</v>
       </c>
       <c r="C29" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1464,10 +1465,10 @@
         <v>44</v>
       </c>
       <c r="C30" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1478,10 +1479,10 @@
         <v>46</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1492,10 +1493,10 @@
         <v>11</v>
       </c>
       <c r="C32" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1506,10 +1507,10 @@
         <v>13</v>
       </c>
       <c r="C33" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1517,13 +1518,13 @@
         <v>84</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C34" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1531,24 +1532,24 @@
         <v>85</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C35" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="28" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C36" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>110</v>
@@ -1556,30 +1557,30 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C37" s="33" t="s">
         <v>103</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="28" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B38" s="24" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1587,13 +1588,13 @@
         <v>89</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="C39" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1601,10 +1602,10 @@
         <v>90</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="C40" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>109</v>
@@ -1615,41 +1616,41 @@
         <v>91</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="C41" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="B42" s="24" t="s">
-        <v>12</v>
+      <c r="B42" s="25" t="s">
+        <v>19</v>
       </c>
       <c r="C42" s="33" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="29" t="s">
+      <c r="A43" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="B43" s="25" t="s">
-        <v>19</v>
+      <c r="B43" s="24" t="s">
+        <v>21</v>
       </c>
       <c r="C43" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1657,7 +1658,7 @@
         <v>94</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C44" s="33" t="s">
         <v>103</v>
@@ -1671,13 +1672,13 @@
         <v>95</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C45" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1685,13 +1686,13 @@
         <v>96</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C46" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1699,13 +1700,13 @@
         <v>97</v>
       </c>
       <c r="B47" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C47" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1713,13 +1714,13 @@
         <v>98</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C48" s="33" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1727,10 +1728,10 @@
         <v>99</v>
       </c>
       <c r="B49" s="24" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C49" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>110</v>
@@ -1741,32 +1742,18 @@
         <v>100</v>
       </c>
       <c r="B50" s="24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C50" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="B51" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="C51" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B64">
-    <sortCondition ref="A2:A64"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B63">
+    <sortCondition ref="A2:A63"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>